<commit_message>
Update 4 loss penalties and previous elo adjustments
</commit_message>
<xml_diff>
--- a/Input Data/Conferences.xlsx
+++ b/Input Data/Conferences.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/580bce16df9ec0bf/Documents/Navigate/CFP Simulator/Input Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="99" documentId="8_{5517F0AA-22C3-49B4-BB71-DB5778D18CCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64385A99-E4CF-4D67-A745-E8F39ECC2FCF}"/>
+  <xr:revisionPtr revIDLastSave="111" documentId="8_{5517F0AA-22C3-49B4-BB71-DB5778D18CCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DC8F4C2-AA64-47DB-9B5C-044EFC890ADE}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D05DAB30-B7C0-4384-BC9A-5B31BC32F4BB}"/>
   </bookViews>
@@ -572,10 +572,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -879,7 +875,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E135" sqref="E135"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>